<commit_message>
- AIDER: fichier de définition des groupes mis à jour.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@19251 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="0" windowWidth="31515" windowHeight="16965" tabRatio="311"/>
+    <workbookView xWindow="13305" yWindow="45" windowWidth="13230" windowHeight="30585" tabRatio="311" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Groupes" sheetId="1" r:id="rId1"/>
     <sheet name="Territorialité" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Groupes!$M$1:$M$677</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="1956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3666" uniqueCount="1961">
   <si>
     <t>Autres</t>
   </si>
@@ -5888,6 +5889,21 @@
   </si>
   <si>
     <t>Catéchumènes 2010-13-15</t>
+  </si>
+  <si>
+    <t>Fonctions</t>
+  </si>
+  <si>
+    <t>Membre du bureau</t>
+  </si>
+  <si>
+    <t>Répondant</t>
+  </si>
+  <si>
+    <t>Responsable budgétaire</t>
+  </si>
+  <si>
+    <t>Boursier</t>
   </si>
 </sst>
 </file>
@@ -6214,7 +6230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6662,6 +6678,7 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7072,9 +7089,9 @@
   </sheetPr>
   <dimension ref="A1:AS677"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A352" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K325" sqref="K325"/>
+      <selection pane="topRight" activeCell="K96" sqref="K96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.125" defaultRowHeight="15" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
@@ -7260,7 +7277,7 @@
       <c r="AR4" s="7"/>
       <c r="AS4" s="7"/>
     </row>
-    <row r="5" spans="1:45" s="8" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="129">
         <v>10000</v>
       </c>
@@ -7317,7 +7334,7 @@
       <c r="AR5" s="32"/>
       <c r="AS5" s="32"/>
     </row>
-    <row r="6" spans="1:45" s="8" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="129">
         <v>11000</v>
       </c>
@@ -7374,7 +7391,7 @@
       <c r="AR6" s="32"/>
       <c r="AS6" s="32"/>
     </row>
-    <row r="7" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>11100</v>
       </c>
@@ -7402,7 +7419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>11110</v>
       </c>
@@ -7439,7 +7456,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>11120</v>
       </c>
@@ -7475,7 +7492,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="10" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>11130</v>
       </c>
@@ -7511,7 +7528,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="11" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>11140</v>
       </c>
@@ -7547,7 +7564,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="12" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
         <v>11150</v>
       </c>
@@ -7583,7 +7600,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>11160</v>
       </c>
@@ -7619,7 +7636,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A14" s="19">
         <v>11200</v>
       </c>
@@ -7642,7 +7659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
         <v>11210</v>
       </c>
@@ -7678,7 +7695,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="16" spans="1:45" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
         <v>11220</v>
       </c>
@@ -7714,7 +7731,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>11230</v>
       </c>
@@ -7750,7 +7767,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>11240</v>
       </c>
@@ -7786,7 +7803,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>11250</v>
       </c>
@@ -7822,7 +7839,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>11260</v>
       </c>
@@ -7858,7 +7875,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A21" s="19">
         <v>11300</v>
       </c>
@@ -7881,7 +7898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>11310</v>
       </c>
@@ -7917,7 +7934,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
         <v>11320</v>
       </c>
@@ -7953,7 +7970,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>11330</v>
       </c>
@@ -7989,7 +8006,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A25" s="19">
         <v>11340</v>
       </c>
@@ -8025,7 +8042,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
         <v>11350</v>
       </c>
@@ -8061,7 +8078,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A27" s="19">
         <v>11360</v>
       </c>
@@ -8097,7 +8114,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
         <v>11400</v>
       </c>
@@ -8120,7 +8137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
         <v>11410</v>
       </c>
@@ -8156,7 +8173,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A30" s="19">
         <v>11420</v>
       </c>
@@ -8192,7 +8209,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A31" s="19">
         <v>11430</v>
       </c>
@@ -8227,7 +8244,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A32" s="19">
         <v>11500</v>
       </c>
@@ -8252,7 +8269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A33" s="19">
         <v>11510</v>
       </c>
@@ -8288,7 +8305,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A34" s="19">
         <v>11520</v>
       </c>
@@ -8324,7 +8341,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A35" s="19">
         <v>11530</v>
       </c>
@@ -8359,7 +8376,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A36" s="19">
         <v>11540</v>
       </c>
@@ -8394,7 +8411,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A37" s="19">
         <v>11600</v>
       </c>
@@ -8414,7 +8431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A38" s="19">
         <v>11610</v>
       </c>
@@ -8449,7 +8466,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A39" s="19">
         <v>11620</v>
       </c>
@@ -8484,7 +8501,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A40" s="19">
         <v>11630</v>
       </c>
@@ -8519,7 +8536,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
         <v>11700</v>
       </c>
@@ -8539,7 +8556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A42" s="19">
         <v>11710</v>
       </c>
@@ -8568,7 +8585,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A43" s="19">
         <v>11720</v>
       </c>
@@ -8597,7 +8614,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
         <v>11730</v>
       </c>
@@ -8626,7 +8643,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A45" s="19">
         <v>11740</v>
       </c>
@@ -8655,7 +8672,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A46" s="19">
         <v>11750</v>
       </c>
@@ -8672,7 +8689,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A47" s="19">
         <v>11800</v>
       </c>
@@ -8692,7 +8709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A48" s="19">
         <v>11810</v>
       </c>
@@ -8721,7 +8738,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A49" s="19">
         <v>11820</v>
       </c>
@@ -8750,7 +8767,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A50" s="19">
         <v>11830</v>
       </c>
@@ -8779,7 +8796,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A51" s="19">
         <v>11840</v>
       </c>
@@ -8808,7 +8825,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A52" s="19">
         <v>11850</v>
       </c>
@@ -8837,7 +8854,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A53" s="19">
         <v>11900</v>
       </c>
@@ -8857,7 +8874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A54" s="19">
         <v>11910</v>
       </c>
@@ -8886,7 +8903,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A55" s="19">
         <v>11920</v>
       </c>
@@ -8915,7 +8932,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="19">
         <v>12000</v>
       </c>
@@ -8935,7 +8952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A57" s="19">
         <v>12010</v>
       </c>
@@ -8965,7 +8982,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A58" s="19">
         <v>12020</v>
       </c>
@@ -8983,7 +9000,7 @@
       </c>
       <c r="L58" s="113"/>
     </row>
-    <row r="59" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A59" s="19">
         <v>12030</v>
       </c>
@@ -9001,7 +9018,7 @@
       </c>
       <c r="L59" s="113"/>
     </row>
-    <row r="60" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A60" s="19">
         <v>12040</v>
       </c>
@@ -9031,7 +9048,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A61" s="19">
         <v>12100</v>
       </c>
@@ -9052,7 +9069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A62" s="19">
         <v>12110</v>
       </c>
@@ -9070,7 +9087,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A63" s="19">
         <v>12120</v>
       </c>
@@ -9088,7 +9105,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A64" s="19">
         <v>12130</v>
       </c>
@@ -9106,7 +9123,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A65" s="19">
         <v>12140</v>
       </c>
@@ -9124,7 +9141,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A66" s="19">
         <v>12200</v>
       </c>
@@ -9145,7 +9162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A67" s="19">
         <v>12210</v>
       </c>
@@ -9163,7 +9180,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A68" s="19">
         <v>12220</v>
       </c>
@@ -9181,7 +9198,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A69" s="19">
         <v>12230</v>
       </c>
@@ -9199,7 +9216,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A70" s="19">
         <v>12300</v>
       </c>
@@ -9220,7 +9237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A71" s="19">
         <v>12310</v>
       </c>
@@ -9238,7 +9255,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A72" s="19">
         <v>12320</v>
       </c>
@@ -9256,7 +9273,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="19">
         <v>12400</v>
       </c>
@@ -9277,7 +9294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A74" s="19">
         <v>12410</v>
       </c>
@@ -9295,7 +9312,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A75" s="19">
         <v>12420</v>
       </c>
@@ -9313,7 +9330,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A76" s="19">
         <v>12430</v>
       </c>
@@ -9331,7 +9348,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A77" s="19">
         <v>12440</v>
       </c>
@@ -9349,7 +9366,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A78" s="19">
         <v>12500</v>
       </c>
@@ -9370,7 +9387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A79" s="19">
         <v>12510</v>
       </c>
@@ -9388,7 +9405,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A80" s="19">
         <v>12520</v>
       </c>
@@ -9406,7 +9423,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A81" s="19">
         <v>12530</v>
       </c>
@@ -9424,7 +9441,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A82" s="19">
         <v>12540</v>
       </c>
@@ -9442,7 +9459,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A83" s="19">
         <v>12550</v>
       </c>
@@ -9460,7 +9477,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A84" s="19">
         <v>12560</v>
       </c>
@@ -9478,7 +9495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A85" s="19">
         <v>12570</v>
       </c>
@@ -9496,7 +9513,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A86" s="19">
         <v>12600</v>
       </c>
@@ -9517,7 +9534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A87" s="19">
         <v>12610</v>
       </c>
@@ -9535,7 +9552,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="88" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A88" s="19">
         <v>12620</v>
       </c>
@@ -9553,7 +9570,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A89" s="19">
         <v>12630</v>
       </c>
@@ -9571,7 +9588,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A90" s="19">
         <v>12640</v>
       </c>
@@ -9589,7 +9606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A91" s="19">
         <v>12700</v>
       </c>
@@ -9610,7 +9627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A92" s="19">
         <v>12710</v>
       </c>
@@ -9628,7 +9645,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A93" s="19">
         <v>12720</v>
       </c>
@@ -9646,7 +9663,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="94" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A94" s="19">
         <v>12800</v>
       </c>
@@ -9690,7 +9707,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="95" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A95" s="19">
         <v>12810</v>
       </c>
@@ -9735,7 +9752,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="96" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:25" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A96" s="130">
         <v>15000</v>
       </c>
@@ -9756,7 +9773,7 @@
       <c r="K96" s="22"/>
       <c r="M96" s="47"/>
     </row>
-    <row r="97" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A97" s="19">
         <v>15100</v>
       </c>
@@ -9773,7 +9790,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A98" s="19">
         <v>15110</v>
       </c>
@@ -9805,7 +9822,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A99" s="19">
         <v>15120</v>
       </c>
@@ -9837,7 +9854,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A100" s="19">
         <v>15130</v>
       </c>
@@ -9870,7 +9887,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A101" s="19">
         <v>15200</v>
       </c>
@@ -9887,7 +9904,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A102" s="19">
         <v>15210</v>
       </c>
@@ -9920,7 +9937,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A103" s="19">
         <v>15220</v>
       </c>
@@ -9953,7 +9970,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A104" s="19">
         <v>15230</v>
       </c>
@@ -9986,7 +10003,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A105" s="19">
         <v>15240</v>
       </c>
@@ -10019,7 +10036,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A106" s="19">
         <v>15250</v>
       </c>
@@ -10052,7 +10069,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A107" s="19">
         <v>15260</v>
       </c>
@@ -10085,7 +10102,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A108" s="19">
         <v>15270</v>
       </c>
@@ -10117,7 +10134,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A109" s="19">
         <v>15280</v>
       </c>
@@ -10149,7 +10166,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A110" s="19">
         <v>15290</v>
       </c>
@@ -10181,7 +10198,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A111" s="19">
         <v>15300</v>
       </c>
@@ -10214,7 +10231,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A112" s="19">
         <v>15310</v>
       </c>
@@ -10247,7 +10264,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A113" s="19">
         <v>15320</v>
       </c>
@@ -10280,7 +10297,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A114" s="19">
         <v>15330</v>
       </c>
@@ -10313,7 +10330,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A115" s="19">
         <v>15340</v>
       </c>
@@ -10346,7 +10363,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A116" s="19">
         <v>15350</v>
       </c>
@@ -10379,7 +10396,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A117" s="19">
         <v>15360</v>
       </c>
@@ -10411,7 +10428,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A118" s="19">
         <v>15370</v>
       </c>
@@ -10444,7 +10461,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A119" s="19">
         <v>15380</v>
       </c>
@@ -10477,7 +10494,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A120" s="19">
         <v>15390</v>
       </c>
@@ -10510,7 +10527,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A121" s="19">
         <v>15500</v>
       </c>
@@ -10527,7 +10544,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A122" s="19">
         <v>15510</v>
       </c>
@@ -10560,7 +10577,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A123" s="19">
         <v>15520</v>
       </c>
@@ -10593,7 +10610,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A124" s="19">
         <v>15530</v>
       </c>
@@ -10626,7 +10643,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A125" s="19">
         <v>15540</v>
       </c>
@@ -10659,7 +10676,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A126" s="19">
         <v>15550</v>
       </c>
@@ -10692,7 +10709,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A127" s="19">
         <v>15560</v>
       </c>
@@ -10725,7 +10742,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A128" s="19">
         <v>15570</v>
       </c>
@@ -10758,7 +10775,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="129" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A129" s="19">
         <v>15580</v>
       </c>
@@ -10791,7 +10808,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="130" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A130" s="19">
         <v>15590</v>
       </c>
@@ -10824,7 +10841,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="131" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A131" s="19">
         <v>15600</v>
       </c>
@@ -10857,7 +10874,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A132" s="19">
         <v>15610</v>
       </c>
@@ -10890,7 +10907,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A133" s="19">
         <v>15620</v>
       </c>
@@ -10923,7 +10940,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A134" s="19">
         <v>15630</v>
       </c>
@@ -10956,7 +10973,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="135" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A135" s="19">
         <v>15700</v>
       </c>
@@ -10973,7 +10990,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="136" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A136" s="19">
         <v>15710</v>
       </c>
@@ -10999,7 +11016,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="137" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A137" s="19">
         <v>15720</v>
       </c>
@@ -11025,7 +11042,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="138" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A138" s="19">
         <v>15800</v>
       </c>
@@ -11048,7 +11065,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="139" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A139" s="19">
         <v>15810</v>
       </c>
@@ -11073,7 +11090,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="140" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:25" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A140" s="130">
         <v>16000</v>
       </c>
@@ -11094,7 +11111,7 @@
       <c r="K140" s="22"/>
       <c r="M140" s="47"/>
     </row>
-    <row r="141" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="19">
         <v>16010</v>
       </c>
@@ -11120,7 +11137,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="142" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A142" s="19">
         <v>16020</v>
       </c>
@@ -11140,7 +11157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A143" s="19">
         <v>16100</v>
       </c>
@@ -11166,7 +11183,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="144" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A144" s="19">
         <v>16110</v>
       </c>
@@ -11186,7 +11203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:27" ht="14.1" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:27" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="130">
         <v>20000</v>
       </c>
@@ -11207,7 +11224,7 @@
       <c r="K145" s="25"/>
       <c r="M145" s="48"/>
     </row>
-    <row r="146" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A146" s="130">
         <v>21000</v>
       </c>
@@ -11228,7 +11245,7 @@
       <c r="K146" s="22"/>
       <c r="M146" s="47"/>
     </row>
-    <row r="147" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A147" s="19">
         <v>21100</v>
       </c>
@@ -11245,7 +11262,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="148" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A148" s="19">
         <v>21110</v>
       </c>
@@ -11274,7 +11291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A149" s="19">
         <v>21120</v>
       </c>
@@ -11309,7 +11326,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="150" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A150" s="19">
         <v>21130</v>
       </c>
@@ -11344,7 +11361,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="151" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A151" s="19">
         <v>21140</v>
       </c>
@@ -11379,7 +11396,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="152" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A152" s="19">
         <v>21150</v>
       </c>
@@ -11414,7 +11431,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="153" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A153" s="19">
         <v>21160</v>
       </c>
@@ -11449,7 +11466,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="154" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A154" s="19">
         <v>21170</v>
       </c>
@@ -11484,7 +11501,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="155" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A155" s="19">
         <v>21180</v>
       </c>
@@ -11519,7 +11536,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="156" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A156" s="19">
         <v>21190</v>
       </c>
@@ -11554,7 +11571,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="157" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A157" s="19">
         <v>21200</v>
       </c>
@@ -11589,7 +11606,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="158" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A158" s="19">
         <v>21210</v>
       </c>
@@ -11624,7 +11641,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="159" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A159" s="19">
         <v>21220</v>
       </c>
@@ -11659,7 +11676,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="160" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A160" s="19">
         <v>21230</v>
       </c>
@@ -11694,7 +11711,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="161" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A161" s="19">
         <v>21240</v>
       </c>
@@ -11729,7 +11746,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="162" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A162" s="19">
         <v>21250</v>
       </c>
@@ -11767,7 +11784,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="163" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A163" s="19">
         <v>21260</v>
       </c>
@@ -11805,7 +11822,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="164" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A164" s="19">
         <v>21300</v>
       </c>
@@ -11822,7 +11839,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="165" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A165" s="19">
         <v>21310</v>
       </c>
@@ -11860,7 +11877,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="166" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A166" s="19">
         <v>21320</v>
       </c>
@@ -11898,7 +11915,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="167" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A167" s="19">
         <v>21330</v>
       </c>
@@ -11933,7 +11950,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="168" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A168" s="19">
         <v>21340</v>
       </c>
@@ -11971,7 +11988,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="169" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A169" s="19">
         <v>21350</v>
       </c>
@@ -12009,7 +12026,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="170" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A170" s="19">
         <v>21360</v>
       </c>
@@ -12047,7 +12064,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="171" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A171" s="19">
         <v>21370</v>
       </c>
@@ -12085,7 +12102,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="172" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A172" s="19">
         <v>21380</v>
       </c>
@@ -12123,7 +12140,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="173" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A173" s="19">
         <v>21400</v>
       </c>
@@ -12141,7 +12158,7 @@
       </c>
       <c r="J173" s="122"/>
     </row>
-    <row r="174" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A174" s="19">
         <v>21410</v>
       </c>
@@ -12179,7 +12196,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="175" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A175" s="19">
         <v>21420</v>
       </c>
@@ -12217,7 +12234,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="176" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A176" s="19">
         <v>21430</v>
       </c>
@@ -12255,7 +12272,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="177" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A177" s="19">
         <v>21440</v>
       </c>
@@ -12293,7 +12310,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="178" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A178" s="19">
         <v>21450</v>
       </c>
@@ -12331,7 +12348,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="179" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A179" s="19">
         <v>21460</v>
       </c>
@@ -12369,7 +12386,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="180" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A180" s="19">
         <v>21470</v>
       </c>
@@ -12407,7 +12424,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="181" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A181" s="19">
         <v>21480</v>
       </c>
@@ -12445,7 +12462,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="182" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A182" s="19">
         <v>21490</v>
       </c>
@@ -12483,7 +12500,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="183" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A183" s="19">
         <v>21600</v>
       </c>
@@ -12500,7 +12517,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="184" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A184" s="19">
         <v>21610</v>
       </c>
@@ -12532,7 +12549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A185" s="19">
         <v>21620</v>
       </c>
@@ -12564,7 +12581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A186" s="19">
         <v>21630</v>
       </c>
@@ -12596,7 +12613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:27" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A187" s="130">
         <v>22000</v>
       </c>
@@ -12617,7 +12634,7 @@
       <c r="K187" s="22"/>
       <c r="M187" s="47"/>
     </row>
-    <row r="188" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A188" s="19">
         <v>22100</v>
       </c>
@@ -12644,7 +12661,7 @@
       <c r="V188" s="70"/>
       <c r="W188" s="76"/>
     </row>
-    <row r="189" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A189" s="19">
         <v>22110</v>
       </c>
@@ -12679,7 +12696,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="190" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A190" s="19">
         <v>22120</v>
       </c>
@@ -12704,7 +12721,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="191" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A191" s="19">
         <v>22130</v>
       </c>
@@ -12729,7 +12746,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="192" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A192" s="19">
         <v>22140</v>
       </c>
@@ -12748,7 +12765,7 @@
       <c r="L192" s="104"/>
       <c r="M192" s="10"/>
     </row>
-    <row r="193" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A193" s="19">
         <v>22150</v>
       </c>
@@ -12780,7 +12797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A194" s="19">
         <v>22160</v>
       </c>
@@ -12797,7 +12814,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="195" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A195" s="19">
         <v>22200</v>
       </c>
@@ -12814,7 +12831,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="196" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A196" s="19">
         <v>22210</v>
       </c>
@@ -12846,7 +12863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="197" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A197" s="19">
         <v>22220</v>
       </c>
@@ -12866,7 +12883,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="198" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A198" s="19">
         <v>22230</v>
       </c>
@@ -12901,7 +12918,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="199" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A199" s="19">
         <v>22240</v>
       </c>
@@ -12928,7 +12945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A200" s="19">
         <v>22250</v>
       </c>
@@ -12954,7 +12971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A201" s="19">
         <v>22260</v>
       </c>
@@ -12990,7 +13007,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="202" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A202" s="19">
         <v>22270</v>
       </c>
@@ -13020,7 +13037,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="203" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A203" s="19">
         <v>22300</v>
       </c>
@@ -13049,7 +13066,7 @@
       <c r="V203" s="70"/>
       <c r="W203" s="76"/>
     </row>
-    <row r="204" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A204" s="19">
         <v>22310</v>
       </c>
@@ -13086,7 +13103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A205" s="19">
         <v>22320</v>
       </c>
@@ -13105,7 +13122,7 @@
       <c r="L205" s="115"/>
       <c r="M205" s="49"/>
     </row>
-    <row r="206" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A206" s="19">
         <v>22330</v>
       </c>
@@ -13136,7 +13153,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="207" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A207" s="19">
         <v>22340</v>
       </c>
@@ -13165,7 +13182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A208" s="19">
         <v>22350</v>
       </c>
@@ -13195,7 +13212,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="209" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A209" s="19">
         <v>22360</v>
       </c>
@@ -13227,7 +13244,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="210" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A210" s="19">
         <v>22370</v>
       </c>
@@ -13257,7 +13274,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="211" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A211" s="19">
         <v>22380</v>
       </c>
@@ -13280,7 +13297,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="212" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A212" s="19">
         <v>22400</v>
       </c>
@@ -13303,7 +13320,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="213" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A213" s="19">
         <v>22410</v>
       </c>
@@ -13329,7 +13346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A214" s="19">
         <v>22420</v>
       </c>
@@ -13349,7 +13366,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="215" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A215" s="19">
         <v>22430</v>
       </c>
@@ -13378,7 +13395,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="216" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:27" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A216" s="19">
         <v>22440</v>
       </c>
@@ -13406,7 +13423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A217" s="19">
         <v>22450</v>
       </c>
@@ -13440,7 +13457,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="218" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A218" s="19">
         <v>22500</v>
       </c>
@@ -13458,7 +13475,7 @@
       </c>
       <c r="L218" s="104"/>
     </row>
-    <row r="219" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A219" s="19">
         <v>22510</v>
       </c>
@@ -13492,7 +13509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A220" s="19">
         <v>22520</v>
       </c>
@@ -13515,7 +13532,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="221" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A221" s="19">
         <v>22600</v>
       </c>
@@ -13533,7 +13550,7 @@
       </c>
       <c r="M221" s="10"/>
     </row>
-    <row r="222" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A222" s="19">
         <v>22610</v>
       </c>
@@ -13565,7 +13582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A223" s="19">
         <v>22620</v>
       </c>
@@ -13589,7 +13606,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="224" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A224" s="19">
         <v>22700</v>
       </c>
@@ -13606,7 +13623,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="225" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A225" s="19">
         <v>22710</v>
       </c>
@@ -13638,7 +13655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A226" s="19">
         <v>22720</v>
       </c>
@@ -13661,7 +13678,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="227" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:25" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A227" s="130">
         <v>23000</v>
       </c>
@@ -13683,7 +13700,7 @@
       <c r="L227" s="115"/>
       <c r="M227" s="50"/>
     </row>
-    <row r="228" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A228" s="19">
         <v>23100</v>
       </c>
@@ -13710,7 +13727,7 @@
       <c r="V228" s="70"/>
       <c r="W228" s="76"/>
     </row>
-    <row r="229" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A229" s="19">
         <v>23110</v>
       </c>
@@ -13746,7 +13763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A230" s="19">
         <v>23120</v>
       </c>
@@ -13770,7 +13787,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="231" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A231" s="19">
         <v>23200</v>
       </c>
@@ -13798,7 +13815,7 @@
       <c r="V231" s="70"/>
       <c r="W231" s="76"/>
     </row>
-    <row r="232" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A232" s="19">
         <v>23210</v>
       </c>
@@ -13835,7 +13852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A233" s="19">
         <v>23220</v>
       </c>
@@ -13859,7 +13876,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="234" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A234" s="19">
         <v>23300</v>
       </c>
@@ -13887,7 +13904,7 @@
       <c r="V234" s="70"/>
       <c r="W234" s="76"/>
     </row>
-    <row r="235" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A235" s="19">
         <v>23310</v>
       </c>
@@ -13923,7 +13940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A236" s="19">
         <v>23320</v>
       </c>
@@ -13947,7 +13964,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="237" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A237" s="19">
         <v>23400</v>
       </c>
@@ -13975,7 +13992,7 @@
       <c r="V237" s="70"/>
       <c r="W237" s="76"/>
     </row>
-    <row r="238" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A238" s="19">
         <v>23410</v>
       </c>
@@ -14011,7 +14028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="239" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A239" s="19">
         <v>23420</v>
       </c>
@@ -14035,7 +14052,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="240" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:25" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A240" s="130">
         <v>24000</v>
       </c>
@@ -14056,7 +14073,7 @@
       <c r="K240" s="22"/>
       <c r="M240" s="47"/>
     </row>
-    <row r="241" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A241" s="19">
         <v>24100</v>
       </c>
@@ -14078,7 +14095,7 @@
       <c r="P241" s="58"/>
       <c r="Q241" s="61"/>
     </row>
-    <row r="242" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A242" s="19">
         <v>24110</v>
       </c>
@@ -14096,7 +14113,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="243" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:25" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A243" s="19">
         <v>24120</v>
       </c>
@@ -14122,7 +14139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:25" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A244" s="19">
         <v>24130</v>
       </c>
@@ -14148,7 +14165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A245" s="19">
         <v>24140</v>
       </c>
@@ -14165,7 +14182,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="246" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:25" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A246" s="19">
         <v>24150</v>
       </c>
@@ -14191,7 +14208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:25" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A247" s="19">
         <v>24160</v>
       </c>
@@ -14217,7 +14234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A248" s="19">
         <v>24200</v>
       </c>
@@ -14235,7 +14252,7 @@
       </c>
       <c r="M248" s="46"/>
     </row>
-    <row r="249" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A249" s="19">
         <v>24210</v>
       </c>
@@ -14253,7 +14270,7 @@
       </c>
       <c r="M249" s="46"/>
     </row>
-    <row r="250" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:25" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A250" s="19">
         <v>24220</v>
       </c>
@@ -14279,7 +14296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:25" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A251" s="19">
         <v>24230</v>
       </c>
@@ -14305,7 +14322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:25" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A252" s="130">
         <v>25000</v>
       </c>
@@ -14326,7 +14343,7 @@
       <c r="K252" s="22"/>
       <c r="M252" s="47"/>
     </row>
-    <row r="253" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:25" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A253" s="19">
         <v>25100</v>
       </c>
@@ -14343,7 +14360,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="254" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A254" s="19">
         <v>25110</v>
       </c>
@@ -14366,7 +14383,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="255" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A255" s="19">
         <v>25120</v>
       </c>
@@ -14389,7 +14406,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="256" spans="1:25" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:25" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A256" s="19">
         <v>25130</v>
       </c>
@@ -14412,7 +14429,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="257" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A257" s="19">
         <v>25140</v>
       </c>
@@ -14435,7 +14452,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="258" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A258" s="19">
         <v>25150</v>
       </c>
@@ -14458,7 +14475,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="259" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A259" s="19">
         <v>25200</v>
       </c>
@@ -14476,7 +14493,7 @@
       </c>
       <c r="K259" s="14"/>
     </row>
-    <row r="260" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A260" s="19">
         <v>25210</v>
       </c>
@@ -14499,7 +14516,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="261" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A261" s="19">
         <v>25300</v>
       </c>
@@ -14517,7 +14534,7 @@
       </c>
       <c r="K261" s="14"/>
     </row>
-    <row r="262" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A262" s="19">
         <v>25310</v>
       </c>
@@ -14540,7 +14557,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="263" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A263" s="19">
         <v>25400</v>
       </c>
@@ -14558,7 +14575,7 @@
       </c>
       <c r="K263" s="14"/>
     </row>
-    <row r="264" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A264" s="19">
         <v>25410</v>
       </c>
@@ -14581,7 +14598,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="265" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A265" s="19">
         <v>25500</v>
       </c>
@@ -14599,7 +14616,7 @@
       </c>
       <c r="K265" s="14"/>
     </row>
-    <row r="266" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A266" s="19">
         <v>25510</v>
       </c>
@@ -14622,7 +14639,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="267" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A267" s="19">
         <v>25600</v>
       </c>
@@ -14640,7 +14657,7 @@
       </c>
       <c r="K267" s="14"/>
     </row>
-    <row r="268" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A268" s="19">
         <v>25610</v>
       </c>
@@ -14663,7 +14680,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="269" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A269" s="19">
         <v>25700</v>
       </c>
@@ -14681,7 +14698,7 @@
       </c>
       <c r="K269" s="14"/>
     </row>
-    <row r="270" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A270" s="19">
         <v>25710</v>
       </c>
@@ -14704,7 +14721,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="271" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A271" s="19">
         <v>25800</v>
       </c>
@@ -14721,7 +14738,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="272" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A272" s="19">
         <v>25810</v>
       </c>
@@ -14747,7 +14764,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="273" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A273" s="19">
         <v>25820</v>
       </c>
@@ -14770,7 +14787,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="274" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A274" s="19">
         <v>25900</v>
       </c>
@@ -14788,7 +14805,7 @@
       </c>
       <c r="K274" s="14"/>
     </row>
-    <row r="275" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A275" s="19">
         <v>25910</v>
       </c>
@@ -14811,7 +14828,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="276" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A276" s="19">
         <v>26000</v>
       </c>
@@ -14829,7 +14846,7 @@
       </c>
       <c r="K276" s="14"/>
     </row>
-    <row r="277" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A277" s="19">
         <v>26010</v>
       </c>
@@ -14852,7 +14869,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="278" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A278" s="19">
         <v>26020</v>
       </c>
@@ -14875,7 +14892,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="279" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A279" s="19">
         <v>26100</v>
       </c>
@@ -14892,7 +14909,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="280" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A280" s="19">
         <v>26110</v>
       </c>
@@ -14915,7 +14932,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="281" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:27" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A281" s="19">
         <v>26200</v>
       </c>
@@ -14932,7 +14949,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="282" spans="1:27" ht="14.1" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:27" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A282" s="19">
         <v>26210</v>
       </c>
@@ -24353,7 +24370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
@@ -24901,4 +24918,172 @@
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="155" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Remplacé AiderGroupDef.NodeType par deux propriétés SubgroupsAllowed et MembersAllowed qui sont nettement plus explicites qui correspondent en gros au notion de définition feuille et de définition noeud. On laisse complêtement tomber la notion de définition racine qui ne servait à rien. Cela permet donc par exemple d'avoir des définitions qui étaient racine avant d'avoir des membres, ce qui n'était pas le cas. - Supprimé GroupNodeType qui ne servait plus à rien. - Adaptations dans les procédures d'imporatations des définition des groupes. - Adaptations dans les tests unitaires.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20164 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3810" uniqueCount="1958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="1958">
   <si>
     <t>Autres</t>
   </si>
@@ -7129,8 +7129,8 @@
   <dimension ref="A1:AS677"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C161" sqref="C161"/>
+      <pane ySplit="4" topLeftCell="A576" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A595" sqref="A595:XFD595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.125" defaultRowHeight="15" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
@@ -11683,9 +11683,7 @@
         <v>564</v>
       </c>
       <c r="AB147" s="98"/>
-      <c r="AC147" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC147" s="143"/>
       <c r="AD147" s="136"/>
     </row>
     <row r="148" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11723,9 +11721,7 @@
         <v>565</v>
       </c>
       <c r="AB148" s="98"/>
-      <c r="AC148" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC148" s="143"/>
       <c r="AD148" s="136"/>
     </row>
     <row r="149" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11763,9 +11759,7 @@
         <v>566</v>
       </c>
       <c r="AB149" s="98"/>
-      <c r="AC149" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC149" s="143"/>
       <c r="AD149" s="136"/>
     </row>
     <row r="150" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11803,9 +11797,7 @@
         <v>567</v>
       </c>
       <c r="AB150" s="98"/>
-      <c r="AC150" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC150" s="143"/>
       <c r="AD150" s="136"/>
     </row>
     <row r="151" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11843,9 +11835,7 @@
         <v>568</v>
       </c>
       <c r="AB151" s="98"/>
-      <c r="AC151" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC151" s="143"/>
       <c r="AD151" s="136"/>
     </row>
     <row r="152" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11883,9 +11873,7 @@
         <v>569</v>
       </c>
       <c r="AB152" s="98"/>
-      <c r="AC152" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC152" s="143"/>
       <c r="AD152" s="136"/>
     </row>
     <row r="153" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11923,9 +11911,7 @@
         <v>570</v>
       </c>
       <c r="AB153" s="98"/>
-      <c r="AC153" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC153" s="143"/>
       <c r="AD153" s="136"/>
     </row>
     <row r="154" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -11963,9 +11949,7 @@
         <v>571</v>
       </c>
       <c r="AB154" s="98"/>
-      <c r="AC154" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC154" s="143"/>
       <c r="AD154" s="136"/>
     </row>
     <row r="155" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12003,9 +11987,7 @@
         <v>572</v>
       </c>
       <c r="AB155" s="98"/>
-      <c r="AC155" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC155" s="143"/>
       <c r="AD155" s="136"/>
     </row>
     <row r="156" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12043,9 +12025,7 @@
         <v>573</v>
       </c>
       <c r="AB156" s="98"/>
-      <c r="AC156" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC156" s="143"/>
       <c r="AD156" s="136"/>
     </row>
     <row r="157" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12083,9 +12063,7 @@
         <v>574</v>
       </c>
       <c r="AB157" s="98"/>
-      <c r="AC157" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC157" s="143"/>
       <c r="AD157" s="136"/>
     </row>
     <row r="158" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12123,9 +12101,7 @@
         <v>575</v>
       </c>
       <c r="AB158" s="98"/>
-      <c r="AC158" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC158" s="143"/>
       <c r="AD158" s="136"/>
     </row>
     <row r="159" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12163,9 +12139,7 @@
         <v>576</v>
       </c>
       <c r="AB159" s="98"/>
-      <c r="AC159" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC159" s="143"/>
       <c r="AD159" s="136"/>
     </row>
     <row r="160" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12206,9 +12180,7 @@
         <v>577</v>
       </c>
       <c r="AB160" s="98"/>
-      <c r="AC160" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC160" s="143"/>
       <c r="AD160" s="136"/>
     </row>
     <row r="161" spans="1:30" ht="14.1" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.2">
@@ -12249,9 +12221,7 @@
         <v>578</v>
       </c>
       <c r="AB161" s="98"/>
-      <c r="AC161" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC161" s="143"/>
       <c r="AD161" s="136"/>
     </row>
     <row r="162" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -13269,9 +13239,7 @@
       <c r="AB189" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC189" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC189" s="143"/>
       <c r="AD189" s="136"/>
     </row>
     <row r="190" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -13374,9 +13342,7 @@
       <c r="AB193" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC193" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC193" s="143"/>
       <c r="AD193" s="136"/>
     </row>
     <row r="194" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -13671,9 +13637,7 @@
       <c r="AB202" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC202" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC202" s="143"/>
       <c r="AD202" s="136"/>
     </row>
     <row r="203" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -13771,9 +13735,7 @@
       <c r="AB205" s="136" t="s">
         <v>628</v>
       </c>
-      <c r="AC205" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC205" s="143"/>
       <c r="AD205" s="136"/>
     </row>
     <row r="206" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -13876,9 +13838,7 @@
       <c r="AB208" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC208" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC208" s="143"/>
       <c r="AD208" s="136"/>
     </row>
     <row r="209" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -13915,9 +13875,7 @@
       <c r="AB209" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC209" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC209" s="143"/>
       <c r="AD209" s="136"/>
     </row>
     <row r="210" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -13952,9 +13910,7 @@
       <c r="AB210" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC210" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC210" s="143"/>
       <c r="AD210" s="136"/>
     </row>
     <row r="211" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -14010,9 +13966,7 @@
       <c r="AB212" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC212" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC212" s="143"/>
       <c r="AD212" s="136"/>
     </row>
     <row r="213" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14094,9 +14048,7 @@
       <c r="AB215" s="136" t="s">
         <v>628</v>
       </c>
-      <c r="AC215" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC215" s="143"/>
       <c r="AD215" s="136"/>
     </row>
     <row r="216" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -14200,9 +14152,7 @@
         <v>348</v>
       </c>
       <c r="AB218" s="136"/>
-      <c r="AC218" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC218" s="143"/>
       <c r="AD218" s="136"/>
     </row>
     <row r="219" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14286,9 +14236,7 @@
         <v>346</v>
       </c>
       <c r="AB221" s="136"/>
-      <c r="AC221" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC221" s="143"/>
       <c r="AD221" s="136"/>
     </row>
     <row r="222" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14371,9 +14319,7 @@
         <v>346</v>
       </c>
       <c r="AB224" s="136"/>
-      <c r="AC224" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC224" s="143"/>
       <c r="AD224" s="136"/>
     </row>
     <row r="225" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14454,9 +14400,7 @@
         <v>346</v>
       </c>
       <c r="AB227" s="136"/>
-      <c r="AC227" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC227" s="143"/>
       <c r="AD227" s="136"/>
     </row>
     <row r="228" spans="1:30" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -14577,9 +14521,7 @@
         <v>346</v>
       </c>
       <c r="AB231" s="136"/>
-      <c r="AC231" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC231" s="143"/>
       <c r="AD231" s="136"/>
     </row>
     <row r="232" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14677,9 +14619,7 @@
         <v>346</v>
       </c>
       <c r="AB234" s="136"/>
-      <c r="AC234" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC234" s="143"/>
       <c r="AD234" s="136"/>
     </row>
     <row r="235" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14776,9 +14716,7 @@
         <v>346</v>
       </c>
       <c r="AB237" s="136"/>
-      <c r="AC237" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC237" s="143"/>
       <c r="AD237" s="136"/>
     </row>
     <row r="238" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -14875,9 +14813,7 @@
         <v>346</v>
       </c>
       <c r="AB240" s="136"/>
-      <c r="AC240" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC240" s="143"/>
       <c r="AD240" s="136"/>
     </row>
     <row r="241" spans="1:30" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -16082,9 +16018,7 @@
       <c r="AB288" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC288" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC288" s="143"/>
       <c r="AD288" s="136"/>
     </row>
     <row r="289" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -16465,9 +16399,7 @@
       <c r="AB300" s="136" t="s">
         <v>898</v>
       </c>
-      <c r="AC300" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC300" s="143"/>
       <c r="AD300" s="136"/>
     </row>
     <row r="301" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16501,9 +16433,7 @@
       <c r="AB301" s="136" t="s">
         <v>898</v>
       </c>
-      <c r="AC301" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC301" s="143"/>
       <c r="AD301" s="136"/>
     </row>
     <row r="302" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16525,9 +16455,7 @@
       <c r="AB302" s="136" t="s">
         <v>898</v>
       </c>
-      <c r="AC302" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC302" s="143"/>
       <c r="AD302" s="136"/>
     </row>
     <row r="303" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16561,9 +16489,7 @@
       <c r="AB303" s="136" t="s">
         <v>898</v>
       </c>
-      <c r="AC303" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC303" s="143"/>
       <c r="AD303" s="136"/>
     </row>
     <row r="304" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -16607,9 +16533,7 @@
       <c r="AB305" s="136" t="s">
         <v>672</v>
       </c>
-      <c r="AC305" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC305" s="143"/>
       <c r="AD305" s="136"/>
     </row>
     <row r="306" spans="1:30" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -16679,9 +16603,7 @@
       <c r="AB308" s="136" t="s">
         <v>906</v>
       </c>
-      <c r="AC308" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC308" s="143"/>
       <c r="AD308" s="136"/>
     </row>
     <row r="309" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16715,9 +16637,7 @@
       <c r="AB309" s="136" t="s">
         <v>906</v>
       </c>
-      <c r="AC309" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC309" s="143"/>
       <c r="AD309" s="136"/>
     </row>
     <row r="310" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16751,9 +16671,7 @@
       <c r="AB310" s="136" t="s">
         <v>906</v>
       </c>
-      <c r="AC310" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC310" s="143"/>
       <c r="AD310" s="136"/>
     </row>
     <row r="311" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16787,9 +16705,7 @@
       <c r="AB311" s="136" t="s">
         <v>906</v>
       </c>
-      <c r="AC311" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC311" s="143"/>
       <c r="AD311" s="136"/>
     </row>
     <row r="312" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -16857,9 +16773,7 @@
       <c r="AB313" s="136" t="s">
         <v>911</v>
       </c>
-      <c r="AC313" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC313" s="143"/>
       <c r="AD313" s="136"/>
     </row>
     <row r="314" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16893,9 +16807,7 @@
       <c r="AB314" s="136" t="s">
         <v>911</v>
       </c>
-      <c r="AC314" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC314" s="143"/>
       <c r="AD314" s="136"/>
     </row>
     <row r="315" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16929,9 +16841,7 @@
       <c r="AB315" s="136" t="s">
         <v>911</v>
       </c>
-      <c r="AC315" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC315" s="143"/>
       <c r="AD315" s="136"/>
     </row>
     <row r="316" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -16965,9 +16875,7 @@
       <c r="AB316" s="136" t="s">
         <v>911</v>
       </c>
-      <c r="AC316" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC316" s="143"/>
       <c r="AD316" s="136"/>
     </row>
     <row r="317" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17001,9 +16909,7 @@
       <c r="AB317" s="136" t="s">
         <v>911</v>
       </c>
-      <c r="AC317" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC317" s="143"/>
       <c r="AD317" s="136"/>
     </row>
     <row r="318" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17037,9 +16943,7 @@
       <c r="AB318" s="136" t="s">
         <v>911</v>
       </c>
-      <c r="AC318" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC318" s="143"/>
       <c r="AD318" s="136"/>
     </row>
     <row r="319" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -17106,9 +17010,7 @@
       <c r="AB320" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC320" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC320" s="143"/>
       <c r="AD320" s="136"/>
     </row>
     <row r="321" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17142,9 +17044,7 @@
       <c r="AB321" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC321" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC321" s="143"/>
       <c r="AD321" s="136"/>
     </row>
     <row r="322" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17178,9 +17078,7 @@
       <c r="AB322" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC322" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC322" s="143"/>
       <c r="AD322" s="136"/>
     </row>
     <row r="323" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17214,9 +17112,7 @@
       <c r="AB323" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC323" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC323" s="143"/>
       <c r="AD323" s="136"/>
     </row>
     <row r="324" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17250,9 +17146,7 @@
       <c r="AB324" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC324" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC324" s="143"/>
       <c r="AD324" s="136"/>
     </row>
     <row r="325" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17287,9 +17181,7 @@
       <c r="AB325" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC325" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC325" s="143"/>
       <c r="AD325" s="136"/>
     </row>
     <row r="326" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17323,9 +17215,7 @@
       <c r="AB326" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC326" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC326" s="143"/>
       <c r="AD326" s="136"/>
     </row>
     <row r="327" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17359,9 +17249,7 @@
       <c r="AB327" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC327" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC327" s="143"/>
       <c r="AD327" s="136"/>
     </row>
     <row r="328" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -17415,9 +17303,7 @@
       <c r="AB329" s="136" t="s">
         <v>672</v>
       </c>
-      <c r="AC329" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC329" s="143"/>
       <c r="AD329" s="136"/>
     </row>
     <row r="330" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -17473,9 +17359,7 @@
       <c r="AB331" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC331" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC331" s="143"/>
       <c r="AD331" s="136"/>
     </row>
     <row r="332" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17509,9 +17393,7 @@
       <c r="AB332" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC332" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC332" s="143"/>
       <c r="AD332" s="136"/>
     </row>
     <row r="333" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17545,9 +17427,7 @@
       <c r="AB333" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC333" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC333" s="143"/>
       <c r="AD333" s="136"/>
     </row>
     <row r="334" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17569,9 +17449,7 @@
       <c r="AB334" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC334" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC334" s="143"/>
       <c r="AD334" s="136"/>
     </row>
     <row r="335" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17605,9 +17483,7 @@
       <c r="AB335" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC335" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC335" s="143"/>
       <c r="AD335" s="136"/>
     </row>
     <row r="336" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17629,9 +17505,7 @@
       <c r="AB336" s="136" t="s">
         <v>672</v>
       </c>
-      <c r="AC336" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC336" s="143"/>
       <c r="AD336" s="136"/>
     </row>
     <row r="337" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17696,9 +17570,7 @@
       <c r="AB338" s="136" t="s">
         <v>672</v>
       </c>
-      <c r="AC338" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC338" s="143"/>
       <c r="AD338" s="136"/>
     </row>
     <row r="339" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -17743,9 +17615,7 @@
       <c r="AB340" s="136" t="s">
         <v>672</v>
       </c>
-      <c r="AC340" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC340" s="143"/>
       <c r="AD340" s="136"/>
     </row>
     <row r="341" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -17811,9 +17681,7 @@
       <c r="AB342" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC342" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC342" s="143"/>
       <c r="AD342" s="136"/>
     </row>
     <row r="343" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -17844,9 +17712,7 @@
       <c r="AB343" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC343" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC343" s="143"/>
       <c r="AD343" s="136"/>
     </row>
     <row r="344" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -17909,9 +17775,7 @@
       <c r="AB345" s="136" t="s">
         <v>672</v>
       </c>
-      <c r="AC345" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC345" s="143"/>
       <c r="AD345" s="136"/>
     </row>
     <row r="346" spans="1:30" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -17994,9 +17858,7 @@
       <c r="AB348" s="136" t="s">
         <v>945</v>
       </c>
-      <c r="AC348" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC348" s="143"/>
       <c r="AD348" s="136"/>
     </row>
     <row r="349" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -18030,9 +17892,7 @@
       <c r="AB349" s="136" t="s">
         <v>945</v>
       </c>
-      <c r="AC349" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC349" s="143"/>
       <c r="AD349" s="136"/>
     </row>
     <row r="350" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -18063,9 +17923,7 @@
       <c r="AB350" s="136" t="s">
         <v>945</v>
       </c>
-      <c r="AC350" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC350" s="143"/>
       <c r="AD350" s="136"/>
     </row>
     <row r="351" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -18093,9 +17951,7 @@
       <c r="AB351" s="136" t="s">
         <v>945</v>
       </c>
-      <c r="AC351" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC351" s="143"/>
       <c r="AD351" s="136"/>
     </row>
     <row r="352" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -18433,7 +18289,9 @@
       <c r="AB365" s="136" t="s">
         <v>1911</v>
       </c>
-      <c r="AC365" s="143"/>
+      <c r="AC365" s="143" t="s">
+        <v>1940</v>
+      </c>
       <c r="AD365" s="136"/>
     </row>
     <row r="366" spans="1:30" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -18807,9 +18665,7 @@
       <c r="AB378" s="136" t="s">
         <v>973</v>
       </c>
-      <c r="AC378" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC378" s="143"/>
       <c r="AD378" s="136"/>
     </row>
     <row r="379" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -18837,9 +18693,7 @@
       <c r="AB379" s="136" t="s">
         <v>973</v>
       </c>
-      <c r="AC379" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC379" s="143"/>
       <c r="AD379" s="136"/>
     </row>
     <row r="380" spans="1:30" ht="14.1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -18895,9 +18749,7 @@
       <c r="AB381" s="136" t="s">
         <v>976</v>
       </c>
-      <c r="AC381" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC381" s="143"/>
       <c r="AD381" s="136"/>
     </row>
     <row r="382" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -18931,9 +18783,7 @@
       <c r="AB382" s="136" t="s">
         <v>976</v>
       </c>
-      <c r="AC382" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC382" s="143"/>
       <c r="AD382" s="136"/>
     </row>
     <row r="383" spans="1:30" ht="14.1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.2">
@@ -18967,9 +18817,7 @@
       <c r="AB383" s="136" t="s">
         <v>976</v>
       </c>
-      <c r="AC383" s="143" t="s">
-        <v>1940</v>
-      </c>
+      <c r="AC383" s="143"/>
       <c r="AD383" s="136"/>
     </row>
     <row r="384" spans="1:30" ht="14.1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
- Ajouté une définition pour le groupe des personnes sans paroisses, au lieu de le rajouter directement lors de l'importation.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20165 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="1958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="1960">
   <si>
     <t>Autres</t>
   </si>
@@ -5896,6 +5896,12 @@
   </si>
   <si>
     <t>0201010115</t>
+  </si>
+  <si>
+    <t>0700000000</t>
+  </si>
+  <si>
+    <t>Personnes sans paroisse</t>
   </si>
 </sst>
 </file>
@@ -7129,8 +7135,8 @@
   <dimension ref="A1:AS677"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A576" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A595" sqref="A595:XFD595"/>
+      <pane ySplit="4" topLeftCell="A645" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G665" sqref="G665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.125" defaultRowHeight="15" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
@@ -7139,7 +7145,7 @@
     <col min="2" max="2" width="10" style="10" customWidth="1"/>
     <col min="3" max="3" width="11.875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.875" style="100" customWidth="1"/>
-    <col min="5" max="5" width="20.875" style="29" customWidth="1"/>
+    <col min="5" max="5" width="36.5" style="29" customWidth="1"/>
     <col min="6" max="6" width="2.875" style="100" customWidth="1"/>
     <col min="7" max="7" width="21.875" style="29" customWidth="1"/>
     <col min="8" max="8" width="2.875" style="104" customWidth="1"/>
@@ -26449,7 +26455,12 @@
       <c r="AD659" s="136"/>
     </row>
     <row r="660" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C660" s="8"/>
+      <c r="C660" s="98" t="s">
+        <v>1958</v>
+      </c>
+      <c r="E660" s="29" t="s">
+        <v>1959</v>
+      </c>
     </row>
     <row r="661" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C661" s="8"/>

</xml_diff>

<commit_message>
- Aider: correctifs pour les données erronées du RCH (encore). - Aider: mise à jour des adresses des paroisses (manque Lausanne 25 et les détails pour Ecublens/Renens/Prilly). - Aider: définitions de groupes (XLSX) avec numéros de la colonne Y synchrones avec numéros de fonctions. - Data.Platform: mise à jour selon données MAT[CH]street Swiss light le plus récent.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20194 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Main/Groupe definition.xlsx
@@ -7141,8 +7141,8 @@
   <dimension ref="A1:AS678"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A420" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G447" sqref="G447"/>
+      <pane ySplit="4" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y91" sqref="Y91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.125" defaultRowHeight="15" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
@@ -9381,7 +9381,7 @@
       </c>
       <c r="K66" s="14"/>
       <c r="Y66" s="77">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AB66" s="136"/>
       <c r="AC66" s="143"/>
@@ -9468,7 +9468,7 @@
       </c>
       <c r="K70" s="14"/>
       <c r="Y70" s="77">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AB70" s="136"/>
       <c r="AC70" s="143"/>
@@ -9534,7 +9534,7 @@
       </c>
       <c r="K73" s="14"/>
       <c r="Y73" s="77">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AB73" s="136"/>
       <c r="AC73" s="143"/>
@@ -9642,7 +9642,7 @@
       </c>
       <c r="K78" s="14"/>
       <c r="Y78" s="77">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AB78" s="136"/>
       <c r="AC78" s="143"/>
@@ -9813,7 +9813,7 @@
       </c>
       <c r="K86" s="14"/>
       <c r="Y86" s="77">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AB86" s="136"/>
       <c r="AC86" s="143"/>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="K91" s="14"/>
       <c r="Y91" s="77">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AB91" s="136"/>
       <c r="AC91" s="143"/>

</xml_diff>